<commit_message>
Fixing some bugs with play-time slider
</commit_message>
<xml_diff>
--- a/errors.xlsx
+++ b/errors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Major code</t>
   </si>
@@ -50,6 +50,15 @@
   <si>
     <t>The _timestamps's index method must have returned integer. 
 Self._timestamps: SortedList</t>
+  </si>
+  <si>
+    <t>Invalid arguments for jump operation.</t>
+  </si>
+  <si>
+    <t>In lyrics editor: column index is neither 0 nor 1.</t>
+  </si>
+  <si>
+    <t>In lyrics editor: column selection can be either 1 or 2</t>
   </si>
 </sst>
 </file>
@@ -402,7 +411,7 @@
   <dimension ref="B2:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,20 +483,32 @@
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>

</xml_diff>